<commit_message>
adding 2023, race #2, 3 & 4
</commit_message>
<xml_diff>
--- a/2023/01-brumov/01-VKCT2023-Brumov.xlsx
+++ b/2023/01-brumov/01-VKCT2023-Brumov.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Předškoláci I" sheetId="1" state="visible" r:id="rId2"/>
@@ -511,10 +511,10 @@
     <t xml:space="preserve">Müllerová Valerie</t>
   </si>
   <si>
-    <t xml:space="preserve">Moravciková Alžběta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moravciková Kateřina</t>
+    <t xml:space="preserve">Moravčíková Alžběta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moravčíková Kateřina</t>
   </si>
   <si>
     <t xml:space="preserve">Starší žačky (2009-2010)</t>
@@ -523,7 +523,7 @@
     <t xml:space="preserve">Vráželová Šárka</t>
   </si>
   <si>
-    <t xml:space="preserve">Chuchmová Justína</t>
+    <t xml:space="preserve">Chuchmová Justýna</t>
   </si>
   <si>
     <t xml:space="preserve">Mladší žáci (2011-2012)</t>
@@ -667,7 +667,7 @@
     <t xml:space="preserve">mtbiker.cz</t>
   </si>
   <si>
-    <t xml:space="preserve">Chudáková Aneta</t>
+    <t xml:space="preserve">Chudárková Aneta</t>
   </si>
   <si>
     <t xml:space="preserve">Ghost team</t>
@@ -691,7 +691,7 @@
     <t xml:space="preserve">Holznerová Petra</t>
   </si>
   <si>
-    <t xml:space="preserve">Fojtikova Staňka</t>
+    <t xml:space="preserve">Fojtíková Stanislava</t>
   </si>
   <si>
     <t xml:space="preserve">Navojná</t>
@@ -3161,8 +3161,8 @@
   </sheetPr>
   <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7585,7 +7585,7 @@
   <dimension ref="A1:K100"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9020,8 +9020,8 @@
   </sheetPr>
   <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12199,7 +12199,7 @@
   <dimension ref="A1:K100"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -23971,7 +23971,7 @@
   <dimension ref="A1:K100"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -27241,7 +27241,7 @@
   <dimension ref="A1:K100"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -28654,7 +28654,7 @@
   <dimension ref="A1:K100"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>